<commit_message>
Agrego actividad clase 16
</commit_message>
<xml_diff>
--- a/Clase_11_Maquinas_Virtuales/JuegosDeMemoria.xlsx
+++ b/Clase_11_Maquinas_Virtuales/JuegosDeMemoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5461adc41206a559/Documentos/CertifiedTechDeveloper/IntroduccionALaInformatica/Cursada/camada8_roberto/Clase_11_Maquinas_Virtuales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24A59F2E-C811-4DFC-B3FC-56BC294D2F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{24A59F2E-C811-4DFC-B3FC-56BC294D2F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA75CAA0-0F40-46B4-8549-2FB6BC071F44}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2280" windowWidth="17280" windowHeight="8964" firstSheet="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FIFO" sheetId="1" r:id="rId1"/>
@@ -517,8 +517,8 @@
   </sheetPr>
   <dimension ref="A1:BC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1395,8 +1395,8 @@
   </sheetPr>
   <dimension ref="A1:CH1000"/>
   <sheetViews>
-    <sheetView topLeftCell="X24" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34:AZ34"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1434,9 @@
         <v>3</v>
       </c>
       <c r="E2" s="22"/>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1446,6 +1449,9 @@
         <v>7</v>
       </c>
       <c r="E3" s="22"/>
+      <c r="F3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1458,6 +1464,9 @@
         <v>4</v>
       </c>
       <c r="E4" s="22"/>
+      <c r="F4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1470,6 +1479,9 @@
         <v>5</v>
       </c>
       <c r="E5" s="22"/>
+      <c r="F5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1482,6 +1494,9 @@
         <v>9</v>
       </c>
       <c r="E6" s="22"/>
+      <c r="F6">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
@@ -1494,6 +1509,9 @@
         <v>8</v>
       </c>
       <c r="E7" s="22"/>
+      <c r="F7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1506,6 +1524,9 @@
         <v>4</v>
       </c>
       <c r="E8" s="22"/>
+      <c r="F8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1518,6 +1539,9 @@
         <v>23</v>
       </c>
       <c r="E9" s="22"/>
+      <c r="F9">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -1530,6 +1554,9 @@
         <v>19</v>
       </c>
       <c r="E10" s="22"/>
+      <c r="F10">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="21"/>

</xml_diff>